<commit_message>
CCDB-314: Delete with children added to import.
</commit_message>
<xml_diff>
--- a/conf-core/src/main/webapp/resources/templates/ccdb_slots.xlsx
+++ b/conf-core/src/main/webapp/resources/templates/ccdb_slots.xlsx
@@ -238,6 +238,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -253,7 +254,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -645,36 +645,36 @@
       <c r="A7" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="7" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="1:11" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="9" t="s">
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="H9" s="10"/>
-      <c r="I9" s="9" t="s">
+      <c r="H9" s="11"/>
+      <c r="I9" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="J9" s="10"/>
-      <c r="K9" s="7" t="s">
+      <c r="J9" s="11"/>
+      <c r="K9" s="8" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="8"/>
+      <c r="A10" s="9"/>
       <c r="B10" s="2" t="s">
         <v>11</v>
       </c>
@@ -702,7 +702,7 @@
       <c r="J10" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="K10" s="8"/>
+      <c r="K10" s="9"/>
     </row>
     <row r="11" spans="1:11" s="3" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6"/>
@@ -743,15 +743,15 @@
     <mergeCell ref="G9:H9"/>
   </mergeCells>
   <dataValidations count="4">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Lorem Ipsum" sqref="G9:H9 J10 K9:K10 H10 I10 I9:J9 F10 G10 B10 B9:F9 C10:E10 A9:A10"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Lorem Ipsum" sqref="G9:H9 J10 K9:K10 H10 I10 I9:J9 F10 G10 C10:E10 B10 B9:F9 A9:A10"/>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I11:I1048576">
       <formula1>"CONTAINS,CONTAINED IN,CONTROLS,CONTROLLED BY,POWERS,POWERED BY"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Lorem Ipsum" sqref="B11:B1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11:B1048576">
       <formula1>"CONTAINER,SLOT"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A11:A1048576">
-      <formula1>"CREATE ENTITY,UPDATE ENTITY,DELETE ENTITY,CREATE PROPERTY,UPDATE PROPERTY,DELETE PROPERTY,CREATE RELATIONSHIP,UPDATE RELATIONSHIP,DELETE RELATIONSHIP,INSTALL DEVICE,UNINSTALL DEVICE"</formula1>
+      <formula1>"CREATE ENTITY,UPDATE ENTITY,DELETE ENTITY,DELETE ENTITY AND CHILDREN,CREATE PROPERTY,UPDATE PROPERTY,DELETE PROPERTY,CREATE RELATIONSHIP,UPDATE RELATIONSHIP,DELETE RELATIONSHIP,INSTALL DEVICE,UNINSTALL DEVICE"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>

</xml_diff>